<commit_message>
update ITOM and Negation
</commit_message>
<xml_diff>
--- a/content/research/ITOM/ITOM_Design.xlsx
+++ b/content/research/ITOM/ITOM_Design.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lzhan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lzhan/Documents/ADMIN/Website/sapere-aude/content/research/ITOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB40C4DA-89A2-1E47-BE97-1303163AF9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5767D62-DDAF-4C43-8BDC-4C003406E433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{C6FD53BC-E490-B041-9AEC-609B35C93EC8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Original Design" sheetId="1" r:id="rId1"/>
+    <sheet name="Pre-Post" sheetId="4" r:id="rId1"/>
     <sheet name="Our Design" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Original Design" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet 4" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="89">
   <si>
     <t xml:space="preserve">A dog letting a ball role behind an occluder by pushing its paw against it. </t>
   </si>
@@ -248,26 +249,59 @@
     <t>不回来</t>
   </si>
   <si>
-    <t>信念</t>
-  </si>
-  <si>
-    <t>实验条件</t>
-  </si>
-  <si>
-    <t>球100f</t>
-  </si>
-  <si>
-    <t>狗100f</t>
-  </si>
-  <si>
-    <t>球100</t>
+    <t>信念状态</t>
+  </si>
+  <si>
+    <t>原初实验</t>
+  </si>
+  <si>
+    <t>01-24 frame</t>
+  </si>
+  <si>
+    <t>25-48 frame</t>
+  </si>
+  <si>
+    <t>狗踢球到挡板中间</t>
+  </si>
+  <si>
+    <t>球移动到挡板左侧</t>
+  </si>
+  <si>
+    <t>49-73 frame</t>
+  </si>
+  <si>
+    <t>球移动到挡板后侧中央</t>
+  </si>
+  <si>
+    <t>实验控制</t>
+  </si>
+  <si>
+    <t>移动</t>
+  </si>
+  <si>
+    <t>狗 (24)</t>
+  </si>
+  <si>
+    <t>挡板倒掉</t>
+  </si>
+  <si>
+    <t>73-241 frame</t>
+  </si>
+  <si>
+    <t>241-265 frame</t>
+  </si>
+  <si>
+    <t>球 (24+24)</t>
+  </si>
+  <si>
+    <t>狗 (24+24)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,27 +328,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="7" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -324,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -332,19 +345,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,11 +701,263 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B81681-124F-4445-8A91-6FAC90F3104E}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD69691E-9406-E548-AF8F-263A569EA910}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" thickTop="1">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
+    <sortCondition ref="A2:A9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64888A3A-32E5-434E-9E8E-2D39BF6FF296}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1011,169 +1306,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD69691E-9406-E548-AF8F-263A569EA910}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73568E8-1441-2243-BD48-B13160732DE0}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD8"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>